<commit_message>
modified:   _posts/2024-04-09-nvda-portfolio-tips.md modified:   assets/nvda04092024returns.png modified:   nvidia04092024returnprofile.xlsx
</commit_message>
<xml_diff>
--- a/nvidia04092024returnprofile.xlsx
+++ b/nvidia04092024returnprofile.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Max Djafari\Documents\GitHub\DemonEyesShmoney.github.io\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{13B77125-E32B-4CC1-8980-58594C5CBCEF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{89FEF829-18D6-4FB6-882F-957B8A74A450}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1545" yWindow="3195" windowWidth="21600" windowHeight="11295" xr2:uid="{6A46B53B-6F33-4ECD-B84E-3EF29547D4EB}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{6A46B53B-6F33-4ECD-B84E-3EF29547D4EB}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -562,7 +562,7 @@
   <dimension ref="A1:L28"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G17" sqref="G17"/>
+      <selection activeCell="G18" sqref="G18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -680,10 +680,10 @@
         <v>950</v>
       </c>
       <c r="E3">
-        <v>13</v>
+        <v>3</v>
       </c>
       <c r="F3" s="2">
-        <v>4.62</v>
+        <v>3.85</v>
       </c>
       <c r="G3" s="2">
         <f>(C3-D3)*100</f>
@@ -691,22 +691,22 @@
       </c>
       <c r="H3" s="3">
         <f t="shared" si="0"/>
-        <v>6500</v>
+        <v>1500</v>
       </c>
       <c r="I3" s="4">
         <f t="shared" si="1"/>
-        <v>494</v>
+        <v>345</v>
       </c>
       <c r="J3" s="5">
         <f t="shared" ref="J3:J8" si="2">(F3*E3)*100</f>
-        <v>6006</v>
+        <v>1155</v>
       </c>
       <c r="K3" s="2">
         <v>4.93</v>
       </c>
       <c r="L3" s="6">
         <f t="shared" ref="L3:L8" si="3">(K3*E3)*100</f>
-        <v>6409</v>
+        <v>1479</v>
       </c>
     </row>
     <row r="4" spans="1:12" x14ac:dyDescent="0.25">
@@ -982,19 +982,19 @@
     <row r="15" spans="1:12" x14ac:dyDescent="0.25">
       <c r="I15" s="3">
         <f>SUM(H2:H8)</f>
-        <v>23000</v>
+        <v>18000</v>
       </c>
       <c r="J15" s="4">
         <f>SUM(I2:I9)</f>
-        <v>7275.6</v>
+        <v>7126.6</v>
       </c>
       <c r="K15" s="5">
         <f>SUM(J2:J9)</f>
-        <v>24576</v>
+        <v>19725</v>
       </c>
       <c r="L15" s="6">
         <f>SUM(L2:L9)</f>
-        <v>28612</v>
+        <v>23682</v>
       </c>
     </row>
     <row r="28" spans="11:11" x14ac:dyDescent="0.25">

</xml_diff>